<commit_message>
updated hours and work on menu still need to add back button
</commit_message>
<xml_diff>
--- a/Documentation_Project2/TimeAccounting_EECS448project2.xlsx
+++ b/Documentation_Project2/TimeAccounting_EECS448project2.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\miria\Desktop\EECS448_Project2\Documentation_Project2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aidan\Desktop\ku\junior spring\EECS 448Projects\EECS448_Project2\Documentation_Project2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0D87F2B0-98B2-44C1-B4D8-E1F9C34F2505}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9642A66-BE0E-439F-B3F5-DA9A1FE5B9AF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="915" yWindow="518" windowWidth="12938" windowHeight="12067" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="228" windowWidth="18060" windowHeight="10416" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -665,14 +665,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="108" zoomScaleNormal="93" workbookViewId="0">
-      <selection activeCell="P9" sqref="P9"/>
+    <sheetView tabSelected="1" zoomScale="108" zoomScaleNormal="93" workbookViewId="0">
+      <selection activeCell="M13" sqref="M13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6875" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="12.69921875" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="22.1875" customWidth="1"/>
-    <col min="2" max="26" width="7.6875" customWidth="1"/>
+    <col min="1" max="1" width="22.19921875" customWidth="1"/>
+    <col min="2" max="26" width="7.69921875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="14.25" customHeight="1">
@@ -716,7 +716,7 @@
       </c>
       <c r="S1" s="62">
         <f>R3+R4+R5+R6+R7+R8+R9+R10+R11+R12+R13</f>
-        <v>1.5520833333333335</v>
+        <v>2.010416666666667</v>
       </c>
     </row>
     <row r="2" spans="1:20" ht="14.25" customHeight="1">
@@ -1008,8 +1008,12 @@
       <c r="K11" s="52">
         <v>0.79166666666666663</v>
       </c>
-      <c r="L11" s="53"/>
-      <c r="M11" s="53"/>
+      <c r="L11" s="53">
+        <v>0.79166666666666663</v>
+      </c>
+      <c r="M11" s="53">
+        <v>0.83333333333333337</v>
+      </c>
       <c r="N11" s="54"/>
       <c r="O11" s="54"/>
       <c r="P11" s="22">
@@ -1020,7 +1024,7 @@
       </c>
       <c r="R11" s="47">
         <f>(E11-D11)+(I11-H11)+(K11-J11)+(M11-L11)+(O11-N11)+(Q11-P11)</f>
-        <v>0.84097222222222223</v>
+        <v>0.88263888888888897</v>
       </c>
     </row>
     <row r="12" spans="1:20" ht="14.25" customHeight="1">
@@ -1047,8 +1051,12 @@
       <c r="K12" s="52">
         <v>0.83333333333333337</v>
       </c>
-      <c r="L12" s="53"/>
-      <c r="M12" s="53"/>
+      <c r="L12" s="53">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="M12" s="53">
+        <v>0.875</v>
+      </c>
       <c r="N12" s="54"/>
       <c r="O12" s="54"/>
       <c r="P12" s="22">
@@ -1059,7 +1067,7 @@
       </c>
       <c r="R12" s="47">
         <f t="shared" si="1"/>
-        <v>0.45833333333333331</v>
+        <v>0.79166666666666674</v>
       </c>
     </row>
     <row r="13" spans="1:20" ht="14.25" customHeight="1">
@@ -1080,8 +1088,12 @@
       <c r="K13" s="52">
         <v>0.58333333333333337</v>
       </c>
-      <c r="L13" s="53"/>
-      <c r="M13" s="53"/>
+      <c r="L13" s="53">
+        <v>0.79166666666666663</v>
+      </c>
+      <c r="M13" s="53">
+        <v>0.875</v>
+      </c>
       <c r="N13" s="54"/>
       <c r="O13" s="54"/>
       <c r="P13" s="22">
@@ -1092,7 +1104,7 @@
       </c>
       <c r="R13" s="47">
         <f t="shared" si="1"/>
-        <v>0.1666666666666668</v>
+        <v>0.25000000000000017</v>
       </c>
     </row>
     <row r="14" spans="1:20" ht="14.25" customHeight="1">
@@ -1147,7 +1159,7 @@
       <c r="R18" s="33"/>
       <c r="S18" s="43">
         <f>(M3-L3)+(M4-L4)+(M5-L5)+(M6-L6)+(M7-L7)+(M8-L8)+(M9-L9)+(M10-L10)+(M11-L11)+(M12-L12)+(M13-L13)+(E3-D3)+(E4-D4)+(E5-D5)+(E6-D6)+(E7-D7)+(E8-D8)+(E9-D9)+(E10-D10)+(E11-D11)+(E12-D12)+(E13-D13)</f>
-        <v>0.21875000000000017</v>
+        <v>0.67708333333333359</v>
       </c>
     </row>
     <row r="19" spans="1:19" ht="14.25" customHeight="1">
@@ -1216,7 +1228,7 @@
       <c r="R26" s="33"/>
       <c r="S26" s="43">
         <f>(M3-L3)+(M4-L4)+(M5-L5)+(M6-L6)+(M7-L7)+(M8-L8)+(M9-L9)+(M10-L10)+(M11-L11)+(M12-L12)+(M13-L13)</f>
-        <v>0</v>
+        <v>0.45833333333333348</v>
       </c>
     </row>
     <row r="27" spans="1:19" ht="14.25" customHeight="1">

</xml_diff>

<commit_message>
add final times to time accounting
</commit_message>
<xml_diff>
--- a/Documentation_Project2/TimeAccounting_EECS448project2.xlsx
+++ b/Documentation_Project2/TimeAccounting_EECS448project2.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aidan\Desktop\ku\junior spring\EECS 448Projects\EECS448_Project2\Documentation_Project2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\miria\Desktop\EECS448_Project2\Documentation_Project2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9642A66-BE0E-439F-B3F5-DA9A1FE5B9AF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{188FE960-A657-420C-B227-E6DA2FABA5A7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="228" windowWidth="18060" windowHeight="10416" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="180" yWindow="638" windowWidth="12938" windowHeight="12067" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="32">
   <si>
     <t>TEAM 02</t>
   </si>
@@ -117,6 +117,18 @@
   </si>
   <si>
     <t xml:space="preserve">Zoom </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Design </t>
+  </si>
+  <si>
+    <t>Framework</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Functionality </t>
+  </si>
+  <si>
+    <t>Groupme Conversation</t>
   </si>
 </sst>
 </file>
@@ -665,14 +677,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="108" zoomScaleNormal="93" workbookViewId="0">
-      <selection activeCell="M13" sqref="M13"/>
+    <sheetView tabSelected="1" zoomScale="96" zoomScaleNormal="93" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.69921875" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="12.6875" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="22.19921875" customWidth="1"/>
-    <col min="2" max="26" width="7.69921875" customWidth="1"/>
+    <col min="1" max="1" width="22.1875" customWidth="1"/>
+    <col min="2" max="26" width="7.6875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="14.25" customHeight="1">
@@ -716,7 +728,7 @@
       </c>
       <c r="S1" s="62">
         <f>R3+R4+R5+R6+R7+R8+R9+R10+R11+R12+R13</f>
-        <v>2.010416666666667</v>
+        <v>3.4479166666666674</v>
       </c>
     </row>
     <row r="2" spans="1:20" ht="14.25" customHeight="1">
@@ -936,7 +948,9 @@
       <c r="C9" s="10"/>
       <c r="D9" s="18"/>
       <c r="E9" s="11"/>
-      <c r="F9" s="9"/>
+      <c r="F9" s="9" t="s">
+        <v>28</v>
+      </c>
       <c r="G9" s="10"/>
       <c r="H9" s="21"/>
       <c r="I9" s="21"/>
@@ -944,13 +958,17 @@
       <c r="K9" s="14"/>
       <c r="L9" s="15"/>
       <c r="M9" s="15"/>
-      <c r="N9" s="54"/>
-      <c r="O9" s="54"/>
+      <c r="N9" s="54">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="O9" s="54">
+        <v>0.58333333333333337</v>
+      </c>
       <c r="P9" s="22"/>
       <c r="Q9" s="17"/>
       <c r="R9" s="47">
         <f t="shared" ref="R9:R13" si="1">(E9-D9)+(I9-H9)+(K9-J9)+(M9-L9)+(O9-N9)+(Q9-P9)</f>
-        <v>0</v>
+        <v>4.1666666666666741E-2</v>
       </c>
     </row>
     <row r="10" spans="1:20" ht="14.25" customHeight="1">
@@ -967,10 +985,16 @@
       <c r="E10" s="18">
         <v>0.9375</v>
       </c>
-      <c r="F10" s="9"/>
+      <c r="F10" s="9" t="s">
+        <v>29</v>
+      </c>
       <c r="G10" s="10"/>
-      <c r="H10" s="21"/>
-      <c r="I10" s="21"/>
+      <c r="H10" s="21">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="I10" s="21">
+        <v>0.79166666666666663</v>
+      </c>
       <c r="J10" s="14"/>
       <c r="K10" s="14"/>
       <c r="L10" s="15"/>
@@ -981,7 +1005,7 @@
       <c r="Q10" s="22"/>
       <c r="R10" s="47">
         <f>(E10-D10)+(I10-H10)</f>
-        <v>3.3333333333333326E-2</v>
+        <v>0.24166666666666659</v>
       </c>
     </row>
     <row r="11" spans="1:20" ht="14.25" customHeight="1">
@@ -998,10 +1022,16 @@
       <c r="E11" s="18">
         <v>0.41666666666666669</v>
       </c>
-      <c r="F11" s="51"/>
+      <c r="F11" s="51" t="s">
+        <v>29</v>
+      </c>
       <c r="G11" s="10"/>
-      <c r="H11" s="39"/>
-      <c r="I11" s="39"/>
+      <c r="H11" s="39">
+        <v>0.375</v>
+      </c>
+      <c r="I11" s="39">
+        <v>0.54166666666666663</v>
+      </c>
       <c r="J11" s="52">
         <v>0.25</v>
       </c>
@@ -1014,8 +1044,12 @@
       <c r="M11" s="53">
         <v>0.83333333333333337</v>
       </c>
-      <c r="N11" s="54"/>
-      <c r="O11" s="54"/>
+      <c r="N11" s="54">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="O11" s="54">
+        <v>0.75</v>
+      </c>
       <c r="P11" s="22">
         <v>0.54166666666666663</v>
       </c>
@@ -1024,7 +1058,7 @@
       </c>
       <c r="R11" s="47">
         <f>(E11-D11)+(I11-H11)+(K11-J11)+(M11-L11)+(O11-N11)+(Q11-P11)</f>
-        <v>0.88263888888888897</v>
+        <v>1.0909722222222222</v>
       </c>
     </row>
     <row r="12" spans="1:20" ht="14.25" customHeight="1">
@@ -1041,10 +1075,16 @@
       <c r="E12" s="18">
         <v>0.625</v>
       </c>
-      <c r="F12" s="10"/>
+      <c r="F12" s="10" t="s">
+        <v>30</v>
+      </c>
       <c r="G12" s="10"/>
-      <c r="H12" s="39"/>
-      <c r="I12" s="39"/>
+      <c r="H12" s="39">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="I12" s="39">
+        <v>0.70833333333333337</v>
+      </c>
       <c r="J12" s="52">
         <v>0.58333333333333337</v>
       </c>
@@ -1057,8 +1097,12 @@
       <c r="M12" s="53">
         <v>0.875</v>
       </c>
-      <c r="N12" s="54"/>
-      <c r="O12" s="54"/>
+      <c r="N12" s="54">
+        <v>0.5</v>
+      </c>
+      <c r="O12" s="54">
+        <v>0.875</v>
+      </c>
       <c r="P12" s="22">
         <v>0.41666666666666669</v>
       </c>
@@ -1067,21 +1111,33 @@
       </c>
       <c r="R12" s="47">
         <f t="shared" si="1"/>
-        <v>0.79166666666666674</v>
+        <v>1.416666666666667</v>
       </c>
     </row>
     <row r="13" spans="1:20" ht="14.25" customHeight="1">
       <c r="A13" s="50">
         <v>44269</v>
       </c>
-      <c r="B13" s="10"/>
+      <c r="B13" s="10" t="s">
+        <v>31</v>
+      </c>
       <c r="C13" s="10"/>
-      <c r="D13" s="18"/>
-      <c r="E13" s="18"/>
-      <c r="F13" s="10"/>
+      <c r="D13" s="18">
+        <v>0.5</v>
+      </c>
+      <c r="E13" s="18">
+        <v>0.5625</v>
+      </c>
+      <c r="F13" s="10" t="s">
+        <v>30</v>
+      </c>
       <c r="G13" s="10"/>
-      <c r="H13" s="39"/>
-      <c r="I13" s="39"/>
+      <c r="H13" s="39">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="I13" s="39">
+        <v>0.625</v>
+      </c>
       <c r="J13" s="52">
         <v>0.45833333333333331</v>
       </c>
@@ -1094,8 +1150,12 @@
       <c r="M13" s="53">
         <v>0.875</v>
       </c>
-      <c r="N13" s="54"/>
-      <c r="O13" s="54"/>
+      <c r="N13" s="54">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="O13" s="54">
+        <v>0.625</v>
+      </c>
       <c r="P13" s="22">
         <v>0.66666666666666663</v>
       </c>
@@ -1104,7 +1164,7 @@
       </c>
       <c r="R13" s="47">
         <f t="shared" si="1"/>
-        <v>0.25000000000000017</v>
+        <v>0.60416666666666685</v>
       </c>
     </row>
     <row r="14" spans="1:20" ht="14.25" customHeight="1">
@@ -1125,7 +1185,7 @@
       <c r="R16" s="27"/>
       <c r="S16" s="41">
         <f>(Q3-P3)+(Q4-P4)+(Q5-P5)+(Q6-P6)+(Q7-P7)+(Q8-P8)+(Q9-P9)+(Q10-P10)+(Q11-P11)+(Q12-P12)+(Q13-P13)+(E3-D3)+(E4-D4)+(E5-D5)+(E6-D6)+(E7-D7)+(E8-D8)+(E9-D9)+(E10-D10)+(E11-D11)+(E12-D12)+(E13-D13)</f>
-        <v>0.63541666666666685</v>
+        <v>0.69791666666666685</v>
       </c>
     </row>
     <row r="17" spans="1:19" ht="14.25" customHeight="1">
@@ -1146,7 +1206,7 @@
       <c r="R17" s="31"/>
       <c r="S17" s="42">
         <f>(O3-N3)+(O4-N4)+(O5-N5)+(O6-N6)+(O7-N7)+(O8-N8)+(O9-N9)+(O10-N10)+(O11-N11)+(O12-N12)+(O13-N13)+(E3-D3)+(E4-D4)+(E5-D5)+(E6-D6)+(E7-D7)+(E8-D8)+(E9-D9)+(E10-D10)+(E11-D11)+(E12-D12)+(E13-D13)</f>
-        <v>0.21875000000000017</v>
+        <v>0.82291666666666685</v>
       </c>
     </row>
     <row r="18" spans="1:19" ht="14.25" customHeight="1">
@@ -1159,7 +1219,7 @@
       <c r="R18" s="33"/>
       <c r="S18" s="43">
         <f>(M3-L3)+(M4-L4)+(M5-L5)+(M6-L6)+(M7-L7)+(M8-L8)+(M9-L9)+(M10-L10)+(M11-L11)+(M12-L12)+(M13-L13)+(E3-D3)+(E4-D4)+(E5-D5)+(E6-D6)+(E7-D7)+(E8-D8)+(E9-D9)+(E10-D10)+(E11-D11)+(E12-D12)+(E13-D13)</f>
-        <v>0.67708333333333359</v>
+        <v>0.73958333333333359</v>
       </c>
     </row>
     <row r="19" spans="1:19" ht="14.25" customHeight="1">
@@ -1169,7 +1229,7 @@
       <c r="R19" s="34"/>
       <c r="S19" s="44">
         <f>(K3-J3)+(K4-J4)+(K5-J5)+(K6-J6)+(K7-J7)+(K8-J8)+(K9-J9)+(K10-J10)+(K11-J11)+(K12-J12)+(K13-J13)+(E3-D3)+(E4-D4)+(E5-D5)+(E6-D6)+(E7-D7)+(E8-D8)+(E9-D9)+(E10-D10)+(E11-D11)+(E12-D12)+(E13-D13)</f>
-        <v>1.135416666666667</v>
+        <v>1.197916666666667</v>
       </c>
     </row>
     <row r="20" spans="1:19" ht="14.25" customHeight="1">
@@ -1179,7 +1239,7 @@
       <c r="R20" s="35"/>
       <c r="S20" s="40">
         <f>(I3-H3)+(I4-H4)+(I5-H5)+(I6-H6)+(I7-H7)+(I8-H8)+(I9-H9)+(I10-H10)+(I11-H11)+(I12-H12)+(I13-H13)+(E3-D3)+(E4-D4)+(E5-D5)+(E6-D6)+(E7-D7)+(E8-D8)+(E9-D9)+(E10-D10)+(E11-D11)+(E12-D12)+(E13-D13)</f>
-        <v>0.21875000000000017</v>
+        <v>1.1145833333333335</v>
       </c>
     </row>
     <row r="21" spans="1:19" ht="14.25" customHeight="1">
@@ -1192,7 +1252,7 @@
       <c r="R22" s="38"/>
       <c r="S22" s="46">
         <f>(E3-D3)+(E4-D4)+(E5-D5)+(E6-D6)+(E7-D7)+(E8-D8)+(E9-D9)+(E10-D10)+(E11-D11)+(E12-D12)+(E13-D13)</f>
-        <v>0.21875000000000017</v>
+        <v>0.28125000000000017</v>
       </c>
     </row>
     <row r="23" spans="1:19" ht="14.25" customHeight="1">
@@ -1218,7 +1278,7 @@
       <c r="R25" s="31"/>
       <c r="S25" s="42">
         <f>(O3-N3)+(O4-N4)+(O5-N5)+(O6-N6)+(O7-N7)+(O8-N8)+(O9-N9)+(O10-N10)+(O11-N11)+(O12-N12)+(O13-N13)</f>
-        <v>0</v>
+        <v>0.54166666666666674</v>
       </c>
     </row>
     <row r="26" spans="1:19" ht="14.25" customHeight="1">
@@ -1248,7 +1308,7 @@
       <c r="R28" s="35"/>
       <c r="S28" s="45">
         <f>(I3-H3)+(I4-H4)+(I5-H5)+(I6-H6)+(I7-H7)+(I8-H8)+(I9-H9)+(I10-H10)+(I11-H11)+(I12-H12)+(I13-H13)</f>
-        <v>0</v>
+        <v>0.83333333333333326</v>
       </c>
     </row>
     <row r="29" spans="1:19" ht="14.25" customHeight="1"/>

</xml_diff>